<commit_message>
Login  - Uses the UserName isntead of email.
</commit_message>
<xml_diff>
--- a/Requirements_Karl_Matt.xlsx
+++ b/Requirements_Karl_Matt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr\Documents\BCIT Term 4\COMP4976 - Asp.net\AssignmentOne\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr\Documents\BCIT Term 4\COMP4976 - Asp.net\AssignmentOne\COMP4976ZenithSociety\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Requirement</t>
   </si>
@@ -157,78 +157,6 @@
     <t>Your Visual Studio Solution will contain Two Projects</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF353535"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ZenithDataLib</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF353535"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The first project is a Class Library dedicated to all the Entity Framework data models. This includes the IdentityModels.cs class.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF353535"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ZenithSociety</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF353535"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-solution file must be saved in this directory</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF353535"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ZenithWebSite</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF353535"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-The second project is ASP.NET MVC 5.0 web application.</t>
-    </r>
-  </si>
-  <si>
     <t>Defailed Information</t>
   </si>
   <si>
@@ -714,13 +642,34 @@
   </si>
   <si>
     <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>ZenithSociety
+solution file must be saved in this directory</t>
+  </si>
+  <si>
+    <t>ZenithDataLib
+The first project is a Class Library dedicated to all the Entity Framework data models. This includes the IdentityModels.cs class.</t>
+  </si>
+  <si>
+    <t>ZenithWebSite
+The second project is ASP.NET MVC 5.0 web application.</t>
+  </si>
+  <si>
+    <t>PARTIAL</t>
+  </si>
+  <si>
+    <t>Need to change so that it is auto filled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -750,20 +699,6 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF353535"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF353535"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -883,8 +818,33 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -933,8 +893,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1264,11 +1234,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1276,174 +1263,117 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1455,8 +1385,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1467,9 +1430,76 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="25" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="25" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="25" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1784,7 +1814,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D20" sqref="D20:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1796,329 +1826,343 @@
   <sheetData>
     <row r="1" spans="2:9" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="83"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+    </row>
+    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="84"/>
+      <c r="C4" s="85" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="86"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="46"/>
+    </row>
+    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="84"/>
+      <c r="C5" s="85" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="86"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48"/>
+    </row>
+    <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="71" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
-    </row>
-    <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="65"/>
-    </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-    </row>
-    <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="73"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="67"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
     </row>
     <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
     </row>
     <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="67"/>
+      <c r="D8" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="90"/>
+      <c r="F8" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="91"/>
     </row>
     <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>57</v>
+      <c r="B9" s="71" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="67"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="71"/>
+      <c r="C10" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="67"/>
+      <c r="D10" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="86"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="67"/>
+      <c r="D11" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="86"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
     </row>
     <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="68"/>
+      <c r="C12" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="67"/>
+      <c r="D12" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="86"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
     </row>
     <row r="13" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
-        <v>51</v>
+      <c r="B13" s="69" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="67"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
     </row>
     <row r="14" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="69"/>
       <c r="C14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="10"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="67"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="48"/>
     </row>
     <row r="15" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="69"/>
       <c r="C15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="67"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48"/>
     </row>
     <row r="16" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
+      <c r="B16" s="69"/>
       <c r="C16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="67"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>52</v>
+      <c r="B17" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="74"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="67"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
     </row>
     <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="67"/>
+      <c r="D18" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="92"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
     </row>
     <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="69"/>
       <c r="C19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="75" t="s">
+        <v>98</v>
+      </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="67"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
     </row>
     <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="69"/>
+      <c r="C20" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="65"/>
       <c r="F20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="67"/>
       <c r="F22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="69"/>
+      <c r="C23" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="D23" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="92"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
-        <v>55</v>
+      <c r="B24" s="68" t="s">
+        <v>52</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="74"/>
       <c r="E24" s="8"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2126,11 +2170,11 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="7"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2138,11 +2182,11 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="7"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2150,11 +2194,11 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="7"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2162,13 +2206,13 @@
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
-        <v>54</v>
+      <c r="B28" s="69" t="s">
+        <v>51</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="10"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2176,11 +2220,11 @@
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
+      <c r="B29" s="69"/>
       <c r="C29" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="10"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -2188,11 +2232,11 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
+      <c r="B30" s="69"/>
       <c r="C30" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="73"/>
       <c r="E30" s="10"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2200,11 +2244,11 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="69"/>
+      <c r="C31" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="10"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2212,13 +2256,13 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="70" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="72"/>
       <c r="E32" s="7"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -2226,11 +2270,11 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="23"/>
+      <c r="B33" s="70"/>
       <c r="C33" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="72"/>
       <c r="E33" s="7"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2238,11 +2282,11 @@
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
+      <c r="B34" s="70"/>
       <c r="C34" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="7"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -2250,11 +2294,11 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
+      <c r="B35" s="70"/>
       <c r="C35" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="D35" s="72"/>
       <c r="E35" s="7"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -2262,11 +2306,11 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="23"/>
+      <c r="B36" s="70"/>
       <c r="C36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="8"/>
+      <c r="D36" s="74"/>
       <c r="E36" s="8"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2274,11 +2318,11 @@
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B37" s="23"/>
+      <c r="B37" s="70"/>
       <c r="C37" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="74"/>
       <c r="E37" s="8"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2286,27 +2330,27 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="25" t="s">
+      <c r="B38" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="69"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="50"/>
     </row>
     <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="7"/>
+      <c r="B39" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="72"/>
       <c r="E39" s="8"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2314,11 +2358,11 @@
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B40" s="39"/>
-      <c r="C40" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D40" s="7"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="72"/>
       <c r="E40" s="8"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2326,11 +2370,11 @@
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B41" s="39"/>
-      <c r="C41" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="7"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="72"/>
       <c r="E41" s="8"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -2338,11 +2382,11 @@
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="39"/>
-      <c r="C42" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="7"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="72"/>
       <c r="E42" s="8"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2350,13 +2394,13 @@
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="34" t="s">
-        <v>66</v>
+      <c r="B43" s="62" t="s">
+        <v>63</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="D43" s="73"/>
       <c r="E43" s="11"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2364,11 +2408,11 @@
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B44" s="34"/>
-      <c r="C44" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="10"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="73"/>
       <c r="E44" s="11"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2376,11 +2420,11 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="B45" s="34"/>
+      <c r="B45" s="62"/>
       <c r="C45" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" s="10"/>
+        <v>66</v>
+      </c>
+      <c r="D45" s="73"/>
       <c r="E45" s="11"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2388,11 +2432,11 @@
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="34"/>
+      <c r="B46" s="62"/>
       <c r="C46" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="D46" s="73"/>
       <c r="E46" s="11"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -2400,11 +2444,11 @@
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="34"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D47" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="D47" s="73"/>
       <c r="E47" s="11"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -2412,11 +2456,11 @@
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="2:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="B48" s="34"/>
+      <c r="B48" s="62"/>
       <c r="C48" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="10"/>
+        <v>69</v>
+      </c>
+      <c r="D48" s="73"/>
       <c r="E48" s="11"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -2424,16 +2468,16 @@
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="2:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="36"/>
-      <c r="C49" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="37"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="70"/>
-      <c r="H49" s="70"/>
-      <c r="I49" s="71"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="80"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="52"/>
     </row>
     <row r="50" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
@@ -2445,201 +2489,196 @@
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="62" t="s">
-        <v>74</v>
+      <c r="B52" s="43" t="s">
+        <v>71</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="2:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="42" t="s">
+      <c r="C54" s="32">
+        <v>10</v>
+      </c>
+      <c r="D54" s="33"/>
+    </row>
+    <row r="55" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D53" s="43" t="s">
+      <c r="C55" s="53">
+        <v>4</v>
+      </c>
+      <c r="D55" s="56"/>
+    </row>
+    <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B56" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="54" spans="2:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="44" t="s">
+      <c r="C56" s="54"/>
+      <c r="D56" s="57"/>
+    </row>
+    <row r="57" spans="2:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="45">
-        <v>10</v>
-      </c>
-      <c r="D54" s="46"/>
-    </row>
-    <row r="55" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B55" s="47" t="s">
+      <c r="C57" s="55"/>
+      <c r="D57" s="58"/>
+    </row>
+    <row r="58" spans="2:9" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="C55" s="56">
-        <v>4</v>
-      </c>
-      <c r="D55" s="59"/>
-    </row>
-    <row r="56" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="48" t="s">
+      <c r="C58" s="32">
+        <v>3</v>
+      </c>
+      <c r="D58" s="33"/>
+    </row>
+    <row r="59" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="57"/>
-      <c r="D56" s="60"/>
-    </row>
-    <row r="57" spans="2:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="49" t="s">
+      <c r="C59" s="53">
+        <v>2</v>
+      </c>
+      <c r="D59" s="56"/>
+    </row>
+    <row r="60" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="58"/>
-      <c r="D57" s="61"/>
-    </row>
-    <row r="58" spans="2:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="44" t="s">
+      <c r="C60" s="54"/>
+      <c r="D60" s="57"/>
+    </row>
+    <row r="61" spans="2:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C58" s="45">
-        <v>3</v>
-      </c>
-      <c r="D58" s="46"/>
-    </row>
-    <row r="59" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B59" s="50" t="s">
+      <c r="C61" s="55"/>
+      <c r="D61" s="58"/>
+    </row>
+    <row r="62" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B62" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="56">
+      <c r="C62" s="53">
+        <v>8</v>
+      </c>
+      <c r="D62" s="56"/>
+    </row>
+    <row r="63" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="54"/>
+      <c r="D63" s="57"/>
+    </row>
+    <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B64" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="54"/>
+      <c r="D64" s="57"/>
+    </row>
+    <row r="65" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B65" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="54"/>
+      <c r="D65" s="57"/>
+    </row>
+    <row r="66" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B66" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="54"/>
+      <c r="D66" s="57"/>
+    </row>
+    <row r="67" spans="2:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="54"/>
+      <c r="D67" s="57"/>
+    </row>
+    <row r="68" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B68" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="54"/>
+      <c r="D68" s="57"/>
+    </row>
+    <row r="69" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B69" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="54"/>
+      <c r="D69" s="57"/>
+    </row>
+    <row r="70" spans="2:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="55"/>
+      <c r="D70" s="58"/>
+    </row>
+    <row r="71" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B71" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" s="53">
         <v>2</v>
       </c>
-      <c r="D59" s="59"/>
-    </row>
-    <row r="60" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="57"/>
-      <c r="D60" s="60"/>
-    </row>
-    <row r="61" spans="2:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="61"/>
-    </row>
-    <row r="62" spans="2:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="B62" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" s="56">
-        <v>8</v>
-      </c>
-      <c r="D62" s="59"/>
-    </row>
-    <row r="63" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="57"/>
-      <c r="D63" s="60"/>
-    </row>
-    <row r="64" spans="2:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B64" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C64" s="57"/>
-      <c r="D64" s="60"/>
-    </row>
-    <row r="65" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B65" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="57"/>
-      <c r="D65" s="60"/>
-    </row>
-    <row r="66" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B66" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" s="57"/>
-      <c r="D66" s="60"/>
-    </row>
-    <row r="67" spans="2:4" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="C67" s="57"/>
-      <c r="D67" s="60"/>
-    </row>
-    <row r="68" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B68" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" s="57"/>
-      <c r="D68" s="60"/>
-    </row>
-    <row r="69" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B69" s="48" t="s">
+      <c r="D71" s="56"/>
+    </row>
+    <row r="72" spans="2:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B72" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="C69" s="57"/>
-      <c r="D69" s="60"/>
-    </row>
-    <row r="70" spans="2:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="49" t="s">
+      <c r="C72" s="54"/>
+      <c r="D72" s="57"/>
+    </row>
+    <row r="73" spans="2:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="61"/>
-    </row>
-    <row r="71" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B71" s="50" t="s">
+      <c r="C73" s="55"/>
+      <c r="D73" s="58"/>
+    </row>
+    <row r="74" spans="2:4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="56">
-        <v>2</v>
-      </c>
-      <c r="D71" s="59"/>
-    </row>
-    <row r="72" spans="2:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B72" s="51" t="s">
+      <c r="C74" s="32">
+        <v>1</v>
+      </c>
+      <c r="D74" s="33"/>
+    </row>
+    <row r="75" spans="2:4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C72" s="57"/>
-      <c r="D72" s="60"/>
-    </row>
-    <row r="73" spans="2:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="C73" s="58"/>
-      <c r="D73" s="61"/>
-    </row>
-    <row r="74" spans="2:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="C74" s="45">
-        <v>1</v>
-      </c>
-      <c r="D74" s="46"/>
-    </row>
-    <row r="75" spans="2:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="C75" s="55">
+      <c r="C75" s="42">
         <v>30</v>
       </c>
-      <c r="D75" s="46"/>
+      <c r="D75" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="C62:C70"/>
-    <mergeCell ref="D62:D70"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="B43:B49"/>
@@ -2656,7 +2695,12 @@
     <mergeCell ref="B32:B37"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="C62:C70"/>
+    <mergeCell ref="D62:D70"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="D71:D73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>